<commit_message>
upload quiz excel (2025-11-09T06:51:54.368Z)
</commit_message>
<xml_diff>
--- a/data/quiz/quiz_import.xlsx
+++ b/data/quiz/quiz_import.xlsx
@@ -1,15 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:41000001_{83C8DA7E-F529-A44C-84AD-54B919FDC641}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quiz" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191028"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -6712,8 +6726,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6772,17 +6786,25 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -6820,7 +6842,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -6854,6 +6876,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -6888,9 +6911,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -7063,14 +7087,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J451"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7102,7 +7126,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -7134,7 +7158,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -7166,7 +7190,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="4" spans="1:10">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -7198,7 +7222,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -7230,7 +7254,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -7262,7 +7286,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="7" spans="1:10">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -7294,7 +7318,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="8" spans="1:10">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -7326,7 +7350,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="9" spans="1:10">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -7358,7 +7382,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="10" spans="1:10">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -7390,7 +7414,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="11" spans="1:10">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -7422,7 +7446,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -7454,7 +7478,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="13" spans="1:10">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -7486,7 +7510,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="14" spans="1:10">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -7518,7 +7542,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="15" spans="1:10">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -7550,7 +7574,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -7582,7 +7606,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -7614,7 +7638,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -7646,7 +7670,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -7678,7 +7702,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="20" spans="1:10">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -7710,7 +7734,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="21" spans="1:10">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -7742,7 +7766,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -7774,7 +7798,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -7806,7 +7830,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="24" spans="1:10">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -7838,7 +7862,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="25" spans="1:10">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -7870,7 +7894,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="26" spans="1:10">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -7902,7 +7926,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="27" spans="1:10">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -7934,7 +7958,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="28" spans="1:10">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -7966,7 +7990,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="29" spans="1:10">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -7998,7 +8022,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="30" spans="1:10">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -8030,7 +8054,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -8062,7 +8086,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="32" spans="1:10">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -8094,7 +8118,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="33" spans="1:10">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -8126,7 +8150,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="34" spans="1:10">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -8158,7 +8182,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="35" spans="1:10">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -8190,7 +8214,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="36" spans="1:10">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -8222,7 +8246,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="37" spans="1:10">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -8254,7 +8278,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="38" spans="1:10">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>37</v>
       </c>
@@ -8286,7 +8310,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="39" spans="1:10">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>38</v>
       </c>
@@ -8318,7 +8342,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="40" spans="1:10">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>39</v>
       </c>
@@ -8350,7 +8374,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="41" spans="1:10">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>40</v>
       </c>
@@ -8382,7 +8406,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="42" spans="1:10">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>41</v>
       </c>
@@ -8414,7 +8438,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="43" spans="1:10">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>42</v>
       </c>
@@ -8446,7 +8470,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="44" spans="1:10">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>43</v>
       </c>
@@ -8478,7 +8502,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="45" spans="1:10">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>44</v>
       </c>
@@ -8510,7 +8534,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="46" spans="1:10">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>45</v>
       </c>
@@ -8542,7 +8566,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="47" spans="1:10">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>46</v>
       </c>
@@ -8574,7 +8598,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="48" spans="1:10">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>47</v>
       </c>
@@ -8606,7 +8630,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="49" spans="1:10">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>48</v>
       </c>
@@ -8638,7 +8662,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="50" spans="1:10">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>49</v>
       </c>
@@ -8670,7 +8694,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="51" spans="1:10">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>50</v>
       </c>
@@ -8702,7 +8726,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="52" spans="1:10">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>51</v>
       </c>
@@ -8734,7 +8758,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="53" spans="1:10">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>52</v>
       </c>
@@ -8766,7 +8790,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="54" spans="1:10">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>53</v>
       </c>
@@ -8798,7 +8822,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="55" spans="1:10">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>54</v>
       </c>
@@ -8830,7 +8854,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="56" spans="1:10">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>55</v>
       </c>
@@ -8862,7 +8886,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="57" spans="1:10">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>56</v>
       </c>
@@ -8894,7 +8918,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="58" spans="1:10">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>57</v>
       </c>
@@ -8926,7 +8950,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="59" spans="1:10">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>58</v>
       </c>
@@ -8958,7 +8982,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="60" spans="1:10">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>59</v>
       </c>
@@ -8990,7 +9014,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="61" spans="1:10">
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>60</v>
       </c>
@@ -9022,7 +9046,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="62" spans="1:10">
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>61</v>
       </c>
@@ -9054,7 +9078,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="63" spans="1:10">
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>62</v>
       </c>
@@ -9086,7 +9110,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="64" spans="1:10">
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>63</v>
       </c>
@@ -9118,7 +9142,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="65" spans="1:10">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>64</v>
       </c>
@@ -9150,7 +9174,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="66" spans="1:10">
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>65</v>
       </c>
@@ -9182,7 +9206,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="67" spans="1:10">
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>66</v>
       </c>
@@ -9214,7 +9238,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="68" spans="1:10">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>67</v>
       </c>
@@ -9246,7 +9270,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="69" spans="1:10">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>68</v>
       </c>
@@ -9278,7 +9302,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="70" spans="1:10">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>69</v>
       </c>
@@ -9310,7 +9334,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="71" spans="1:10">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>70</v>
       </c>
@@ -9342,7 +9366,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="72" spans="1:10">
+    <row r="72" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>71</v>
       </c>
@@ -9374,7 +9398,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="73" spans="1:10">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>72</v>
       </c>
@@ -9406,7 +9430,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="74" spans="1:10">
+    <row r="74" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>73</v>
       </c>
@@ -9438,7 +9462,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="75" spans="1:10">
+    <row r="75" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>74</v>
       </c>
@@ -9470,7 +9494,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="76" spans="1:10">
+    <row r="76" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>75</v>
       </c>
@@ -9502,7 +9526,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="77" spans="1:10">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>76</v>
       </c>
@@ -9534,7 +9558,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="78" spans="1:10">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>77</v>
       </c>
@@ -9566,7 +9590,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="79" spans="1:10">
+    <row r="79" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>78</v>
       </c>
@@ -9598,7 +9622,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="80" spans="1:10">
+    <row r="80" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>79</v>
       </c>
@@ -9630,7 +9654,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="81" spans="1:10">
+    <row r="81" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>80</v>
       </c>
@@ -9662,7 +9686,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="82" spans="1:10">
+    <row r="82" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>81</v>
       </c>
@@ -9694,7 +9718,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="83" spans="1:10">
+    <row r="83" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>82</v>
       </c>
@@ -9726,7 +9750,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="84" spans="1:10">
+    <row r="84" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>83</v>
       </c>
@@ -9758,7 +9782,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="85" spans="1:10">
+    <row r="85" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>84</v>
       </c>
@@ -9790,7 +9814,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="86" spans="1:10">
+    <row r="86" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>85</v>
       </c>
@@ -9822,7 +9846,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="87" spans="1:10">
+    <row r="87" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>86</v>
       </c>
@@ -9854,7 +9878,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="88" spans="1:10">
+    <row r="88" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>87</v>
       </c>
@@ -9886,7 +9910,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="89" spans="1:10">
+    <row r="89" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>88</v>
       </c>
@@ -9918,7 +9942,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="90" spans="1:10">
+    <row r="90" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>89</v>
       </c>
@@ -9950,7 +9974,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="91" spans="1:10">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>90</v>
       </c>
@@ -9982,7 +10006,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="92" spans="1:10">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>91</v>
       </c>
@@ -10014,7 +10038,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="93" spans="1:10">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>92</v>
       </c>
@@ -10046,7 +10070,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="94" spans="1:10">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>93</v>
       </c>
@@ -10078,7 +10102,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="95" spans="1:10">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>94</v>
       </c>
@@ -10110,7 +10134,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="96" spans="1:10">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>95</v>
       </c>
@@ -10142,7 +10166,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="97" spans="1:10">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>96</v>
       </c>
@@ -10174,7 +10198,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="98" spans="1:10">
+    <row r="98" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>97</v>
       </c>
@@ -10206,7 +10230,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="99" spans="1:10">
+    <row r="99" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>98</v>
       </c>
@@ -10238,7 +10262,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="100" spans="1:10">
+    <row r="100" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>99</v>
       </c>
@@ -10270,7 +10294,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="101" spans="1:10">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>100</v>
       </c>
@@ -10302,7 +10326,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="102" spans="1:10">
+    <row r="102" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>101</v>
       </c>
@@ -10334,7 +10358,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="103" spans="1:10">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>102</v>
       </c>
@@ -10366,7 +10390,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="104" spans="1:10">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>103</v>
       </c>
@@ -10398,7 +10422,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="105" spans="1:10">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>104</v>
       </c>
@@ -10430,7 +10454,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="106" spans="1:10">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>105</v>
       </c>
@@ -10462,7 +10486,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="107" spans="1:10">
+    <row r="107" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>106</v>
       </c>
@@ -10494,7 +10518,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="108" spans="1:10">
+    <row r="108" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>107</v>
       </c>
@@ -10526,7 +10550,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="109" spans="1:10">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>108</v>
       </c>
@@ -10558,7 +10582,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="110" spans="1:10">
+    <row r="110" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>109</v>
       </c>
@@ -10590,7 +10614,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="111" spans="1:10">
+    <row r="111" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>110</v>
       </c>
@@ -10622,7 +10646,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="112" spans="1:10">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>111</v>
       </c>
@@ -10654,7 +10678,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="113" spans="1:10">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>112</v>
       </c>
@@ -10686,7 +10710,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="114" spans="1:10">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>113</v>
       </c>
@@ -10718,7 +10742,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="115" spans="1:10">
+    <row r="115" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>114</v>
       </c>
@@ -10750,7 +10774,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="116" spans="1:10">
+    <row r="116" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>115</v>
       </c>
@@ -10782,7 +10806,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="117" spans="1:10">
+    <row r="117" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>116</v>
       </c>
@@ -10814,7 +10838,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="118" spans="1:10">
+    <row r="118" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>117</v>
       </c>
@@ -10846,7 +10870,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="119" spans="1:10">
+    <row r="119" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>118</v>
       </c>
@@ -10878,7 +10902,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="120" spans="1:10">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>119</v>
       </c>
@@ -10910,7 +10934,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="121" spans="1:10">
+    <row r="121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>120</v>
       </c>
@@ -10942,7 +10966,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="122" spans="1:10">
+    <row r="122" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>121</v>
       </c>
@@ -10974,7 +10998,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="123" spans="1:10">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>122</v>
       </c>
@@ -11006,7 +11030,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="124" spans="1:10">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>123</v>
       </c>
@@ -11038,7 +11062,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="125" spans="1:10">
+    <row r="125" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>124</v>
       </c>
@@ -11070,7 +11094,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="126" spans="1:10">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>125</v>
       </c>
@@ -11102,7 +11126,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="127" spans="1:10">
+    <row r="127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>126</v>
       </c>
@@ -11134,7 +11158,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="128" spans="1:10">
+    <row r="128" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>127</v>
       </c>
@@ -11166,7 +11190,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="129" spans="1:10">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>128</v>
       </c>
@@ -11198,7 +11222,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="130" spans="1:10">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>129</v>
       </c>
@@ -11230,7 +11254,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="131" spans="1:10">
+    <row r="131" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>130</v>
       </c>
@@ -11262,7 +11286,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="132" spans="1:10">
+    <row r="132" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>131</v>
       </c>
@@ -11294,7 +11318,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="133" spans="1:10">
+    <row r="133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>132</v>
       </c>
@@ -11326,7 +11350,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="134" spans="1:10">
+    <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>133</v>
       </c>
@@ -11358,7 +11382,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="135" spans="1:10">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>134</v>
       </c>
@@ -11390,7 +11414,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="136" spans="1:10">
+    <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>135</v>
       </c>
@@ -11422,7 +11446,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="137" spans="1:10">
+    <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>136</v>
       </c>
@@ -11454,7 +11478,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="138" spans="1:10">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>137</v>
       </c>
@@ -11486,7 +11510,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="139" spans="1:10">
+    <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>138</v>
       </c>
@@ -11518,7 +11542,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="140" spans="1:10">
+    <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>139</v>
       </c>
@@ -11550,7 +11574,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="141" spans="1:10">
+    <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>140</v>
       </c>
@@ -11582,7 +11606,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="142" spans="1:10">
+    <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>141</v>
       </c>
@@ -11614,7 +11638,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="143" spans="1:10">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>142</v>
       </c>
@@ -11646,7 +11670,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="144" spans="1:10">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>143</v>
       </c>
@@ -11678,7 +11702,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="145" spans="1:10">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>144</v>
       </c>
@@ -11710,7 +11734,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="146" spans="1:10">
+    <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>145</v>
       </c>
@@ -11742,7 +11766,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="147" spans="1:10">
+    <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>146</v>
       </c>
@@ -11774,7 +11798,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="148" spans="1:10">
+    <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>147</v>
       </c>
@@ -11806,7 +11830,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="149" spans="1:10">
+    <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>148</v>
       </c>
@@ -11838,7 +11862,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="150" spans="1:10">
+    <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>149</v>
       </c>
@@ -11870,7 +11894,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="151" spans="1:10">
+    <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>150</v>
       </c>
@@ -11902,7 +11926,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="152" spans="1:10">
+    <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>151</v>
       </c>
@@ -11934,7 +11958,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="153" spans="1:10">
+    <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>152</v>
       </c>
@@ -11966,7 +11990,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="154" spans="1:10">
+    <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>153</v>
       </c>
@@ -11998,7 +12022,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="155" spans="1:10">
+    <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>154</v>
       </c>
@@ -12030,7 +12054,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="156" spans="1:10">
+    <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>155</v>
       </c>
@@ -12062,7 +12086,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="157" spans="1:10">
+    <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>156</v>
       </c>
@@ -12094,7 +12118,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="158" spans="1:10">
+    <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>157</v>
       </c>
@@ -12126,7 +12150,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="159" spans="1:10">
+    <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>158</v>
       </c>
@@ -12158,7 +12182,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="160" spans="1:10">
+    <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>159</v>
       </c>
@@ -12190,7 +12214,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="161" spans="1:10">
+    <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>160</v>
       </c>
@@ -12222,7 +12246,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="162" spans="1:10">
+    <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>161</v>
       </c>
@@ -12254,7 +12278,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="163" spans="1:10">
+    <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>162</v>
       </c>
@@ -12286,7 +12310,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="164" spans="1:10">
+    <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>163</v>
       </c>
@@ -12318,7 +12342,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="165" spans="1:10">
+    <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>164</v>
       </c>
@@ -12350,7 +12374,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="166" spans="1:10">
+    <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166">
         <v>165</v>
       </c>
@@ -12382,7 +12406,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="167" spans="1:10">
+    <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167">
         <v>166</v>
       </c>
@@ -12414,7 +12438,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="168" spans="1:10">
+    <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168">
         <v>167</v>
       </c>
@@ -12446,7 +12470,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="169" spans="1:10">
+    <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169">
         <v>168</v>
       </c>
@@ -12478,7 +12502,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="170" spans="1:10">
+    <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170">
         <v>169</v>
       </c>
@@ -12510,7 +12534,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="171" spans="1:10">
+    <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171">
         <v>170</v>
       </c>
@@ -12542,7 +12566,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="172" spans="1:10">
+    <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172">
         <v>171</v>
       </c>
@@ -12574,7 +12598,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="173" spans="1:10">
+    <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173">
         <v>172</v>
       </c>
@@ -12606,7 +12630,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="174" spans="1:10">
+    <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174">
         <v>173</v>
       </c>
@@ -12638,7 +12662,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="175" spans="1:10">
+    <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175">
         <v>174</v>
       </c>
@@ -12670,7 +12694,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="176" spans="1:10">
+    <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176">
         <v>175</v>
       </c>
@@ -12702,7 +12726,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="177" spans="1:10">
+    <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177">
         <v>176</v>
       </c>
@@ -12734,7 +12758,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="178" spans="1:10">
+    <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178">
         <v>177</v>
       </c>
@@ -12766,7 +12790,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="179" spans="1:10">
+    <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179">
         <v>178</v>
       </c>
@@ -12798,7 +12822,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="180" spans="1:10">
+    <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180">
         <v>179</v>
       </c>
@@ -12830,7 +12854,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="181" spans="1:10">
+    <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181">
         <v>180</v>
       </c>
@@ -12862,7 +12886,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="182" spans="1:10">
+    <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182">
         <v>181</v>
       </c>
@@ -12894,7 +12918,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="183" spans="1:10">
+    <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183">
         <v>182</v>
       </c>
@@ -12926,7 +12950,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="184" spans="1:10">
+    <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184">
         <v>183</v>
       </c>
@@ -12958,7 +12982,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="185" spans="1:10">
+    <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185">
         <v>184</v>
       </c>
@@ -12990,7 +13014,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="186" spans="1:10">
+    <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186">
         <v>185</v>
       </c>
@@ -13022,7 +13046,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="187" spans="1:10">
+    <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187">
         <v>186</v>
       </c>
@@ -13054,7 +13078,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="188" spans="1:10">
+    <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188">
         <v>187</v>
       </c>
@@ -13086,7 +13110,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="189" spans="1:10">
+    <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189">
         <v>188</v>
       </c>
@@ -13118,7 +13142,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="190" spans="1:10">
+    <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190">
         <v>189</v>
       </c>
@@ -13150,7 +13174,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="191" spans="1:10">
+    <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191">
         <v>190</v>
       </c>
@@ -13182,7 +13206,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="192" spans="1:10">
+    <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192">
         <v>191</v>
       </c>
@@ -13214,7 +13238,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="193" spans="1:10">
+    <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193">
         <v>192</v>
       </c>
@@ -13246,7 +13270,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="194" spans="1:10">
+    <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194">
         <v>193</v>
       </c>
@@ -13278,7 +13302,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="195" spans="1:10">
+    <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195">
         <v>194</v>
       </c>
@@ -13310,7 +13334,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="196" spans="1:10">
+    <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196">
         <v>195</v>
       </c>
@@ -13342,7 +13366,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="197" spans="1:10">
+    <row r="197" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A197">
         <v>196</v>
       </c>
@@ -13374,7 +13398,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="198" spans="1:10">
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198">
         <v>197</v>
       </c>
@@ -13406,7 +13430,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="199" spans="1:10">
+    <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199">
         <v>198</v>
       </c>
@@ -13438,7 +13462,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="200" spans="1:10">
+    <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200">
         <v>199</v>
       </c>
@@ -13470,7 +13494,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="201" spans="1:10">
+    <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201">
         <v>200</v>
       </c>
@@ -13502,7 +13526,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="202" spans="1:10">
+    <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202">
         <v>201</v>
       </c>
@@ -13534,7 +13558,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="203" spans="1:10">
+    <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203">
         <v>202</v>
       </c>
@@ -13566,7 +13590,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="204" spans="1:10">
+    <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204">
         <v>203</v>
       </c>
@@ -13598,7 +13622,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="205" spans="1:10">
+    <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205">
         <v>204</v>
       </c>
@@ -13630,7 +13654,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="206" spans="1:10">
+    <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206">
         <v>205</v>
       </c>
@@ -13662,7 +13686,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="207" spans="1:10">
+    <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207">
         <v>206</v>
       </c>
@@ -13694,7 +13718,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="208" spans="1:10">
+    <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208">
         <v>207</v>
       </c>
@@ -13726,7 +13750,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="209" spans="1:10">
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A209">
         <v>208</v>
       </c>
@@ -13758,7 +13782,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="210" spans="1:10">
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A210">
         <v>209</v>
       </c>
@@ -13790,7 +13814,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="211" spans="1:10">
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A211">
         <v>210</v>
       </c>
@@ -13822,7 +13846,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="212" spans="1:10">
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A212">
         <v>211</v>
       </c>
@@ -13854,7 +13878,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="213" spans="1:10">
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A213">
         <v>212</v>
       </c>
@@ -13886,7 +13910,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="214" spans="1:10">
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A214">
         <v>213</v>
       </c>
@@ -13918,7 +13942,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="215" spans="1:10">
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A215">
         <v>214</v>
       </c>
@@ -13950,7 +13974,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="216" spans="1:10">
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A216">
         <v>215</v>
       </c>
@@ -13982,7 +14006,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="217" spans="1:10">
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A217">
         <v>216</v>
       </c>
@@ -14014,7 +14038,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="218" spans="1:10">
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A218">
         <v>217</v>
       </c>
@@ -14046,7 +14070,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="219" spans="1:10">
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A219">
         <v>218</v>
       </c>
@@ -14078,7 +14102,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="220" spans="1:10">
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A220">
         <v>219</v>
       </c>
@@ -14110,7 +14134,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="221" spans="1:10">
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A221">
         <v>220</v>
       </c>
@@ -14142,7 +14166,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="222" spans="1:10">
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A222">
         <v>221</v>
       </c>
@@ -14174,7 +14198,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="223" spans="1:10">
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A223">
         <v>222</v>
       </c>
@@ -14206,7 +14230,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="224" spans="1:10">
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A224">
         <v>223</v>
       </c>
@@ -14238,7 +14262,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="225" spans="1:10">
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A225">
         <v>224</v>
       </c>
@@ -14270,7 +14294,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="226" spans="1:10">
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A226">
         <v>225</v>
       </c>
@@ -14302,7 +14326,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="227" spans="1:10">
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A227">
         <v>226</v>
       </c>
@@ -14334,7 +14358,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="228" spans="1:10">
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A228">
         <v>227</v>
       </c>
@@ -14366,7 +14390,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="229" spans="1:10">
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A229">
         <v>228</v>
       </c>
@@ -14398,7 +14422,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="230" spans="1:10">
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A230">
         <v>229</v>
       </c>
@@ -14430,7 +14454,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="231" spans="1:10">
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A231">
         <v>230</v>
       </c>
@@ -14462,7 +14486,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="232" spans="1:10">
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A232">
         <v>231</v>
       </c>
@@ -14494,7 +14518,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="233" spans="1:10">
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A233">
         <v>232</v>
       </c>
@@ -14526,7 +14550,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="234" spans="1:10">
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A234">
         <v>233</v>
       </c>
@@ -14558,7 +14582,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="235" spans="1:10">
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A235">
         <v>234</v>
       </c>
@@ -14590,7 +14614,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="236" spans="1:10">
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A236">
         <v>235</v>
       </c>
@@ -14622,7 +14646,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="237" spans="1:10">
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A237">
         <v>236</v>
       </c>
@@ -14654,7 +14678,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="238" spans="1:10">
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A238">
         <v>237</v>
       </c>
@@ -14686,7 +14710,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="239" spans="1:10">
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A239">
         <v>238</v>
       </c>
@@ -14718,7 +14742,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="240" spans="1:10">
+    <row r="240" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A240">
         <v>239</v>
       </c>
@@ -14750,7 +14774,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="241" spans="1:10">
+    <row r="241" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A241">
         <v>240</v>
       </c>
@@ -14782,7 +14806,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="242" spans="1:10">
+    <row r="242" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A242">
         <v>241</v>
       </c>
@@ -14814,7 +14838,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="243" spans="1:10">
+    <row r="243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A243">
         <v>242</v>
       </c>
@@ -14846,7 +14870,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="244" spans="1:10">
+    <row r="244" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A244">
         <v>243</v>
       </c>
@@ -14878,7 +14902,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="245" spans="1:10">
+    <row r="245" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A245">
         <v>244</v>
       </c>
@@ -14910,7 +14934,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="246" spans="1:10">
+    <row r="246" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A246">
         <v>245</v>
       </c>
@@ -14942,7 +14966,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="247" spans="1:10">
+    <row r="247" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A247">
         <v>246</v>
       </c>
@@ -14974,7 +14998,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="248" spans="1:10">
+    <row r="248" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A248">
         <v>247</v>
       </c>
@@ -15006,7 +15030,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="249" spans="1:10">
+    <row r="249" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A249">
         <v>248</v>
       </c>
@@ -15038,7 +15062,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="250" spans="1:10">
+    <row r="250" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A250">
         <v>249</v>
       </c>
@@ -15070,7 +15094,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="251" spans="1:10">
+    <row r="251" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A251">
         <v>250</v>
       </c>
@@ -15102,7 +15126,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="252" spans="1:10">
+    <row r="252" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A252">
         <v>251</v>
       </c>
@@ -15134,7 +15158,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="253" spans="1:10">
+    <row r="253" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A253">
         <v>252</v>
       </c>
@@ -15166,7 +15190,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="254" spans="1:10">
+    <row r="254" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A254">
         <v>253</v>
       </c>
@@ -15198,7 +15222,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="255" spans="1:10">
+    <row r="255" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A255">
         <v>254</v>
       </c>
@@ -15230,7 +15254,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="256" spans="1:10">
+    <row r="256" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A256">
         <v>255</v>
       </c>
@@ -15262,7 +15286,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="257" spans="1:10">
+    <row r="257" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A257">
         <v>256</v>
       </c>
@@ -15294,7 +15318,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="258" spans="1:10">
+    <row r="258" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A258">
         <v>257</v>
       </c>
@@ -15326,7 +15350,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="259" spans="1:10">
+    <row r="259" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A259">
         <v>258</v>
       </c>
@@ -15358,7 +15382,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="260" spans="1:10">
+    <row r="260" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A260">
         <v>259</v>
       </c>
@@ -15390,7 +15414,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="261" spans="1:10">
+    <row r="261" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A261">
         <v>260</v>
       </c>
@@ -15422,7 +15446,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="262" spans="1:10">
+    <row r="262" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A262">
         <v>261</v>
       </c>
@@ -15454,7 +15478,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="263" spans="1:10">
+    <row r="263" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A263">
         <v>262</v>
       </c>
@@ -15486,7 +15510,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="264" spans="1:10">
+    <row r="264" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A264">
         <v>263</v>
       </c>
@@ -15518,7 +15542,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="265" spans="1:10">
+    <row r="265" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A265">
         <v>264</v>
       </c>
@@ -15550,7 +15574,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="266" spans="1:10">
+    <row r="266" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A266">
         <v>265</v>
       </c>
@@ -15582,7 +15606,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="267" spans="1:10">
+    <row r="267" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A267">
         <v>266</v>
       </c>
@@ -15614,7 +15638,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="268" spans="1:10">
+    <row r="268" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A268">
         <v>267</v>
       </c>
@@ -15646,7 +15670,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="269" spans="1:10">
+    <row r="269" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A269">
         <v>268</v>
       </c>
@@ -15678,7 +15702,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="270" spans="1:10">
+    <row r="270" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A270">
         <v>269</v>
       </c>
@@ -15710,7 +15734,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="271" spans="1:10">
+    <row r="271" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A271">
         <v>270</v>
       </c>
@@ -15742,7 +15766,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="272" spans="1:10">
+    <row r="272" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A272">
         <v>271</v>
       </c>
@@ -15774,7 +15798,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="273" spans="1:10">
+    <row r="273" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A273">
         <v>272</v>
       </c>
@@ -15806,7 +15830,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="274" spans="1:10">
+    <row r="274" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A274">
         <v>273</v>
       </c>
@@ -15838,7 +15862,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="275" spans="1:10">
+    <row r="275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A275">
         <v>274</v>
       </c>
@@ -15870,7 +15894,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="276" spans="1:10">
+    <row r="276" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A276">
         <v>275</v>
       </c>
@@ -15902,7 +15926,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="277" spans="1:10">
+    <row r="277" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A277">
         <v>276</v>
       </c>
@@ -15934,7 +15958,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="278" spans="1:10">
+    <row r="278" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A278">
         <v>277</v>
       </c>
@@ -15966,7 +15990,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="279" spans="1:10">
+    <row r="279" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A279">
         <v>278</v>
       </c>
@@ -15998,7 +16022,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="280" spans="1:10">
+    <row r="280" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A280">
         <v>279</v>
       </c>
@@ -16030,7 +16054,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="281" spans="1:10">
+    <row r="281" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A281">
         <v>280</v>
       </c>
@@ -16062,7 +16086,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="282" spans="1:10">
+    <row r="282" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A282">
         <v>281</v>
       </c>
@@ -16094,7 +16118,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="283" spans="1:10">
+    <row r="283" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A283">
         <v>282</v>
       </c>
@@ -16126,7 +16150,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="284" spans="1:10">
+    <row r="284" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A284">
         <v>283</v>
       </c>
@@ -16158,7 +16182,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="285" spans="1:10">
+    <row r="285" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A285">
         <v>284</v>
       </c>
@@ -16190,7 +16214,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="286" spans="1:10">
+    <row r="286" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A286">
         <v>285</v>
       </c>
@@ -16222,7 +16246,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="287" spans="1:10">
+    <row r="287" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A287">
         <v>286</v>
       </c>
@@ -16254,7 +16278,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="288" spans="1:10">
+    <row r="288" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A288">
         <v>287</v>
       </c>
@@ -16286,7 +16310,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="289" spans="1:10">
+    <row r="289" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A289">
         <v>288</v>
       </c>
@@ -16318,7 +16342,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="290" spans="1:10">
+    <row r="290" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A290">
         <v>289</v>
       </c>
@@ -16350,7 +16374,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="291" spans="1:10">
+    <row r="291" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A291">
         <v>290</v>
       </c>
@@ -16382,7 +16406,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="292" spans="1:10">
+    <row r="292" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A292">
         <v>291</v>
       </c>
@@ -16414,7 +16438,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="293" spans="1:10">
+    <row r="293" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A293">
         <v>292</v>
       </c>
@@ -16446,7 +16470,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="294" spans="1:10">
+    <row r="294" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A294">
         <v>293</v>
       </c>
@@ -16478,7 +16502,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="295" spans="1:10">
+    <row r="295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A295">
         <v>294</v>
       </c>
@@ -16510,7 +16534,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="296" spans="1:10">
+    <row r="296" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A296">
         <v>295</v>
       </c>
@@ -16542,7 +16566,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="297" spans="1:10">
+    <row r="297" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A297">
         <v>296</v>
       </c>
@@ -16574,7 +16598,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="298" spans="1:10">
+    <row r="298" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A298">
         <v>297</v>
       </c>
@@ -16606,7 +16630,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="299" spans="1:10">
+    <row r="299" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A299">
         <v>298</v>
       </c>
@@ -16638,7 +16662,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="300" spans="1:10">
+    <row r="300" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A300">
         <v>299</v>
       </c>
@@ -16670,7 +16694,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="301" spans="1:10">
+    <row r="301" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A301">
         <v>300</v>
       </c>
@@ -16702,7 +16726,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="302" spans="1:10">
+    <row r="302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A302">
         <v>301</v>
       </c>
@@ -16734,7 +16758,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="303" spans="1:10">
+    <row r="303" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A303">
         <v>302</v>
       </c>
@@ -16766,7 +16790,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="304" spans="1:10">
+    <row r="304" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A304">
         <v>303</v>
       </c>
@@ -16798,7 +16822,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="305" spans="1:10">
+    <row r="305" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A305">
         <v>304</v>
       </c>
@@ -16830,7 +16854,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="306" spans="1:10">
+    <row r="306" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A306">
         <v>305</v>
       </c>
@@ -16862,7 +16886,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="307" spans="1:10">
+    <row r="307" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A307">
         <v>306</v>
       </c>
@@ -16894,7 +16918,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="308" spans="1:10">
+    <row r="308" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A308">
         <v>307</v>
       </c>
@@ -16926,7 +16950,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="309" spans="1:10">
+    <row r="309" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A309">
         <v>308</v>
       </c>
@@ -16958,7 +16982,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="310" spans="1:10">
+    <row r="310" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A310">
         <v>309</v>
       </c>
@@ -16990,7 +17014,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="311" spans="1:10">
+    <row r="311" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A311">
         <v>310</v>
       </c>
@@ -17022,7 +17046,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="312" spans="1:10">
+    <row r="312" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A312">
         <v>311</v>
       </c>
@@ -17054,7 +17078,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="313" spans="1:10">
+    <row r="313" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A313">
         <v>312</v>
       </c>
@@ -17086,7 +17110,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="314" spans="1:10">
+    <row r="314" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A314">
         <v>313</v>
       </c>
@@ -17118,7 +17142,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="315" spans="1:10">
+    <row r="315" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A315">
         <v>314</v>
       </c>
@@ -17150,7 +17174,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="316" spans="1:10">
+    <row r="316" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A316">
         <v>315</v>
       </c>
@@ -17182,7 +17206,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="317" spans="1:10">
+    <row r="317" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A317">
         <v>316</v>
       </c>
@@ -17214,7 +17238,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="318" spans="1:10">
+    <row r="318" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A318">
         <v>317</v>
       </c>
@@ -17246,7 +17270,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="319" spans="1:10">
+    <row r="319" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A319">
         <v>318</v>
       </c>
@@ -17278,7 +17302,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="320" spans="1:10">
+    <row r="320" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A320">
         <v>319</v>
       </c>
@@ -17310,7 +17334,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="321" spans="1:10">
+    <row r="321" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A321">
         <v>320</v>
       </c>
@@ -17342,7 +17366,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="322" spans="1:10">
+    <row r="322" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A322">
         <v>321</v>
       </c>
@@ -17374,7 +17398,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="323" spans="1:10">
+    <row r="323" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A323">
         <v>322</v>
       </c>
@@ -17406,7 +17430,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="324" spans="1:10">
+    <row r="324" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A324">
         <v>323</v>
       </c>
@@ -17438,7 +17462,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="325" spans="1:10">
+    <row r="325" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A325">
         <v>324</v>
       </c>
@@ -17470,7 +17494,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="326" spans="1:10">
+    <row r="326" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A326">
         <v>325</v>
       </c>
@@ -17502,7 +17526,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="327" spans="1:10">
+    <row r="327" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A327">
         <v>326</v>
       </c>
@@ -17534,7 +17558,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="328" spans="1:10">
+    <row r="328" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A328">
         <v>327</v>
       </c>
@@ -17566,7 +17590,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="329" spans="1:10">
+    <row r="329" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A329">
         <v>328</v>
       </c>
@@ -17598,7 +17622,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="330" spans="1:10">
+    <row r="330" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A330">
         <v>329</v>
       </c>
@@ -17630,7 +17654,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="331" spans="1:10">
+    <row r="331" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A331">
         <v>330</v>
       </c>
@@ -17662,7 +17686,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="332" spans="1:10">
+    <row r="332" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A332">
         <v>331</v>
       </c>
@@ -17694,7 +17718,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="333" spans="1:10">
+    <row r="333" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A333">
         <v>332</v>
       </c>
@@ -17726,7 +17750,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="334" spans="1:10">
+    <row r="334" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A334">
         <v>333</v>
       </c>
@@ -17758,7 +17782,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="335" spans="1:10">
+    <row r="335" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A335">
         <v>334</v>
       </c>
@@ -17790,7 +17814,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="336" spans="1:10">
+    <row r="336" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A336">
         <v>335</v>
       </c>
@@ -17822,7 +17846,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="337" spans="1:10">
+    <row r="337" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A337">
         <v>336</v>
       </c>
@@ -17854,7 +17878,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="338" spans="1:10">
+    <row r="338" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A338">
         <v>337</v>
       </c>
@@ -17886,7 +17910,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="339" spans="1:10">
+    <row r="339" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A339">
         <v>338</v>
       </c>
@@ -17918,7 +17942,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="340" spans="1:10">
+    <row r="340" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A340">
         <v>339</v>
       </c>
@@ -17950,7 +17974,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="341" spans="1:10">
+    <row r="341" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A341">
         <v>340</v>
       </c>
@@ -17982,7 +18006,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="342" spans="1:10">
+    <row r="342" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A342">
         <v>341</v>
       </c>
@@ -18014,7 +18038,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="343" spans="1:10">
+    <row r="343" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A343">
         <v>342</v>
       </c>
@@ -18046,7 +18070,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="344" spans="1:10">
+    <row r="344" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A344">
         <v>343</v>
       </c>
@@ -18078,7 +18102,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="345" spans="1:10">
+    <row r="345" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A345">
         <v>344</v>
       </c>
@@ -18110,7 +18134,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="346" spans="1:10">
+    <row r="346" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A346">
         <v>345</v>
       </c>
@@ -18142,7 +18166,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="347" spans="1:10">
+    <row r="347" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A347">
         <v>346</v>
       </c>
@@ -18174,7 +18198,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="348" spans="1:10">
+    <row r="348" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A348">
         <v>347</v>
       </c>
@@ -18206,7 +18230,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="349" spans="1:10">
+    <row r="349" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A349">
         <v>348</v>
       </c>
@@ -18238,7 +18262,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="350" spans="1:10">
+    <row r="350" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A350">
         <v>349</v>
       </c>
@@ -18270,7 +18294,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="351" spans="1:10">
+    <row r="351" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A351">
         <v>350</v>
       </c>
@@ -18302,7 +18326,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="352" spans="1:10">
+    <row r="352" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A352">
         <v>351</v>
       </c>
@@ -18334,7 +18358,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="353" spans="1:10">
+    <row r="353" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A353">
         <v>352</v>
       </c>
@@ -18366,7 +18390,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="354" spans="1:10">
+    <row r="354" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A354">
         <v>353</v>
       </c>
@@ -18398,7 +18422,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="355" spans="1:10">
+    <row r="355" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A355">
         <v>354</v>
       </c>
@@ -18430,7 +18454,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="356" spans="1:10">
+    <row r="356" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A356">
         <v>355</v>
       </c>
@@ -18462,7 +18486,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="357" spans="1:10">
+    <row r="357" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A357">
         <v>356</v>
       </c>
@@ -18494,7 +18518,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="358" spans="1:10">
+    <row r="358" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A358">
         <v>357</v>
       </c>
@@ -18526,7 +18550,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="359" spans="1:10">
+    <row r="359" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A359">
         <v>358</v>
       </c>
@@ -18558,7 +18582,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="360" spans="1:10">
+    <row r="360" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A360">
         <v>359</v>
       </c>
@@ -18590,7 +18614,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="361" spans="1:10">
+    <row r="361" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A361">
         <v>360</v>
       </c>
@@ -18622,7 +18646,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="362" spans="1:10">
+    <row r="362" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A362">
         <v>361</v>
       </c>
@@ -18654,7 +18678,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="363" spans="1:10">
+    <row r="363" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A363">
         <v>362</v>
       </c>
@@ -18686,7 +18710,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="364" spans="1:10">
+    <row r="364" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A364">
         <v>363</v>
       </c>
@@ -18718,7 +18742,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="365" spans="1:10">
+    <row r="365" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A365">
         <v>364</v>
       </c>
@@ -18750,7 +18774,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="366" spans="1:10">
+    <row r="366" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A366">
         <v>365</v>
       </c>
@@ -18782,7 +18806,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="367" spans="1:10">
+    <row r="367" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A367">
         <v>366</v>
       </c>
@@ -18814,7 +18838,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="368" spans="1:10">
+    <row r="368" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A368">
         <v>367</v>
       </c>
@@ -18846,7 +18870,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="369" spans="1:10">
+    <row r="369" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A369">
         <v>368</v>
       </c>
@@ -18878,7 +18902,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="370" spans="1:10">
+    <row r="370" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A370">
         <v>369</v>
       </c>
@@ -18910,7 +18934,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="371" spans="1:10">
+    <row r="371" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A371">
         <v>370</v>
       </c>
@@ -18942,7 +18966,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="372" spans="1:10">
+    <row r="372" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A372">
         <v>371</v>
       </c>
@@ -18974,7 +18998,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="373" spans="1:10">
+    <row r="373" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A373">
         <v>372</v>
       </c>
@@ -19006,7 +19030,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="374" spans="1:10">
+    <row r="374" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A374">
         <v>373</v>
       </c>
@@ -19038,7 +19062,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="375" spans="1:10">
+    <row r="375" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A375">
         <v>374</v>
       </c>
@@ -19070,7 +19094,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="376" spans="1:10">
+    <row r="376" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A376">
         <v>375</v>
       </c>
@@ -19102,7 +19126,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="377" spans="1:10">
+    <row r="377" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A377">
         <v>376</v>
       </c>
@@ -19134,7 +19158,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="378" spans="1:10">
+    <row r="378" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A378">
         <v>377</v>
       </c>
@@ -19166,7 +19190,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="379" spans="1:10">
+    <row r="379" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A379">
         <v>378</v>
       </c>
@@ -19198,7 +19222,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="380" spans="1:10">
+    <row r="380" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A380">
         <v>379</v>
       </c>
@@ -19230,7 +19254,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="381" spans="1:10">
+    <row r="381" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A381">
         <v>380</v>
       </c>
@@ -19262,7 +19286,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="382" spans="1:10">
+    <row r="382" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A382">
         <v>381</v>
       </c>
@@ -19294,7 +19318,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="383" spans="1:10">
+    <row r="383" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A383">
         <v>382</v>
       </c>
@@ -19326,7 +19350,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="384" spans="1:10">
+    <row r="384" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A384">
         <v>383</v>
       </c>
@@ -19358,7 +19382,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="385" spans="1:10">
+    <row r="385" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A385">
         <v>384</v>
       </c>
@@ -19390,7 +19414,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="386" spans="1:10">
+    <row r="386" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A386">
         <v>385</v>
       </c>
@@ -19422,7 +19446,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="387" spans="1:10">
+    <row r="387" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A387">
         <v>386</v>
       </c>
@@ -19454,7 +19478,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="388" spans="1:10">
+    <row r="388" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A388">
         <v>387</v>
       </c>
@@ -19486,7 +19510,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="389" spans="1:10">
+    <row r="389" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A389">
         <v>388</v>
       </c>
@@ -19518,7 +19542,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="390" spans="1:10">
+    <row r="390" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A390">
         <v>389</v>
       </c>
@@ -19550,7 +19574,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="391" spans="1:10">
+    <row r="391" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A391">
         <v>390</v>
       </c>
@@ -19582,7 +19606,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="392" spans="1:10">
+    <row r="392" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A392">
         <v>391</v>
       </c>
@@ -19614,7 +19638,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="393" spans="1:10">
+    <row r="393" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A393">
         <v>392</v>
       </c>
@@ -19646,7 +19670,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="394" spans="1:10">
+    <row r="394" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A394">
         <v>393</v>
       </c>
@@ -19678,7 +19702,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="395" spans="1:10">
+    <row r="395" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A395">
         <v>394</v>
       </c>
@@ -19710,7 +19734,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="396" spans="1:10">
+    <row r="396" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A396">
         <v>395</v>
       </c>
@@ -19742,7 +19766,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="397" spans="1:10">
+    <row r="397" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A397">
         <v>396</v>
       </c>
@@ -19774,7 +19798,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="398" spans="1:10">
+    <row r="398" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A398">
         <v>397</v>
       </c>
@@ -19806,7 +19830,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="399" spans="1:10">
+    <row r="399" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A399">
         <v>398</v>
       </c>
@@ -19838,7 +19862,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="400" spans="1:10">
+    <row r="400" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A400">
         <v>399</v>
       </c>
@@ -19870,7 +19894,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="401" spans="1:10">
+    <row r="401" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A401">
         <v>400</v>
       </c>
@@ -19902,7 +19926,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="402" spans="1:10">
+    <row r="402" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A402">
         <v>401</v>
       </c>
@@ -19934,7 +19958,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="403" spans="1:10">
+    <row r="403" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A403">
         <v>402</v>
       </c>
@@ -19966,7 +19990,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="404" spans="1:10">
+    <row r="404" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A404">
         <v>403</v>
       </c>
@@ -19998,7 +20022,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="405" spans="1:10">
+    <row r="405" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A405">
         <v>404</v>
       </c>
@@ -20030,7 +20054,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="406" spans="1:10">
+    <row r="406" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A406">
         <v>405</v>
       </c>
@@ -20062,7 +20086,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="407" spans="1:10">
+    <row r="407" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A407">
         <v>406</v>
       </c>
@@ -20094,7 +20118,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="408" spans="1:10">
+    <row r="408" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A408">
         <v>407</v>
       </c>
@@ -20126,7 +20150,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="409" spans="1:10">
+    <row r="409" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A409">
         <v>408</v>
       </c>
@@ -20158,7 +20182,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="410" spans="1:10">
+    <row r="410" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A410">
         <v>409</v>
       </c>
@@ -20190,7 +20214,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="411" spans="1:10">
+    <row r="411" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A411">
         <v>410</v>
       </c>
@@ -20222,7 +20246,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="412" spans="1:10">
+    <row r="412" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A412">
         <v>411</v>
       </c>
@@ -20254,7 +20278,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="413" spans="1:10">
+    <row r="413" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A413">
         <v>412</v>
       </c>
@@ -20286,7 +20310,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="414" spans="1:10">
+    <row r="414" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A414">
         <v>413</v>
       </c>
@@ -20318,7 +20342,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="415" spans="1:10">
+    <row r="415" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A415">
         <v>414</v>
       </c>
@@ -20350,7 +20374,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="416" spans="1:10">
+    <row r="416" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A416">
         <v>415</v>
       </c>
@@ -20382,7 +20406,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="417" spans="1:10">
+    <row r="417" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A417">
         <v>416</v>
       </c>
@@ -20414,7 +20438,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="418" spans="1:10">
+    <row r="418" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A418">
         <v>417</v>
       </c>
@@ -20446,7 +20470,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="419" spans="1:10">
+    <row r="419" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A419">
         <v>418</v>
       </c>
@@ -20478,7 +20502,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="420" spans="1:10">
+    <row r="420" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A420">
         <v>419</v>
       </c>
@@ -20510,7 +20534,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="421" spans="1:10">
+    <row r="421" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A421">
         <v>420</v>
       </c>
@@ -20542,7 +20566,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="422" spans="1:10">
+    <row r="422" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A422">
         <v>421</v>
       </c>
@@ -20574,7 +20598,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="423" spans="1:10">
+    <row r="423" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A423">
         <v>422</v>
       </c>
@@ -20606,7 +20630,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="424" spans="1:10">
+    <row r="424" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A424">
         <v>423</v>
       </c>
@@ -20638,7 +20662,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="425" spans="1:10">
+    <row r="425" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A425">
         <v>424</v>
       </c>
@@ -20670,7 +20694,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="426" spans="1:10">
+    <row r="426" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A426">
         <v>425</v>
       </c>
@@ -20702,7 +20726,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="427" spans="1:10">
+    <row r="427" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A427">
         <v>426</v>
       </c>
@@ -20734,7 +20758,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="428" spans="1:10">
+    <row r="428" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A428">
         <v>427</v>
       </c>
@@ -20766,7 +20790,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="429" spans="1:10">
+    <row r="429" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A429">
         <v>428</v>
       </c>
@@ -20798,7 +20822,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="430" spans="1:10">
+    <row r="430" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A430">
         <v>429</v>
       </c>
@@ -20830,7 +20854,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="431" spans="1:10">
+    <row r="431" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A431">
         <v>430</v>
       </c>
@@ -20862,7 +20886,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="432" spans="1:10">
+    <row r="432" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A432">
         <v>431</v>
       </c>
@@ -20894,7 +20918,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="433" spans="1:10">
+    <row r="433" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A433">
         <v>432</v>
       </c>
@@ -20926,7 +20950,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="434" spans="1:10">
+    <row r="434" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A434">
         <v>433</v>
       </c>
@@ -20958,7 +20982,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="435" spans="1:10">
+    <row r="435" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A435">
         <v>434</v>
       </c>
@@ -20990,7 +21014,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="436" spans="1:10">
+    <row r="436" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A436">
         <v>435</v>
       </c>
@@ -21022,7 +21046,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="437" spans="1:10">
+    <row r="437" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A437">
         <v>436</v>
       </c>
@@ -21054,7 +21078,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="438" spans="1:10">
+    <row r="438" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A438">
         <v>437</v>
       </c>
@@ -21086,7 +21110,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="439" spans="1:10">
+    <row r="439" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A439">
         <v>438</v>
       </c>
@@ -21118,7 +21142,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="440" spans="1:10">
+    <row r="440" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A440">
         <v>439</v>
       </c>
@@ -21150,7 +21174,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="441" spans="1:10">
+    <row r="441" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A441">
         <v>440</v>
       </c>
@@ -21182,7 +21206,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="442" spans="1:10">
+    <row r="442" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A442">
         <v>441</v>
       </c>
@@ -21214,7 +21238,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="443" spans="1:10">
+    <row r="443" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A443">
         <v>442</v>
       </c>
@@ -21246,7 +21270,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="444" spans="1:10">
+    <row r="444" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A444">
         <v>443</v>
       </c>
@@ -21278,7 +21302,7 @@
         <v>2228</v>
       </c>
     </row>
-    <row r="445" spans="1:10">
+    <row r="445" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A445">
         <v>444</v>
       </c>
@@ -21310,7 +21334,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="446" spans="1:10">
+    <row r="446" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A446">
         <v>445</v>
       </c>
@@ -21342,7 +21366,7 @@
         <v>2229</v>
       </c>
     </row>
-    <row r="447" spans="1:10">
+    <row r="447" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A447">
         <v>446</v>
       </c>
@@ -21374,7 +21398,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="448" spans="1:10">
+    <row r="448" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A448">
         <v>447</v>
       </c>
@@ -21406,7 +21430,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="449" spans="1:10">
+    <row r="449" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A449">
         <v>448</v>
       </c>
@@ -21438,7 +21462,7 @@
         <v>2230</v>
       </c>
     </row>
-    <row r="450" spans="1:10">
+    <row r="450" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A450">
         <v>449</v>
       </c>
@@ -21470,7 +21494,7 @@
         <v>2227</v>
       </c>
     </row>
-    <row r="451" spans="1:10">
+    <row r="451" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A451">
         <v>450</v>
       </c>
@@ -21505,4 +21529,10 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
+<clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
+  <clbl:label id="{0529e95c-c294-4dfa-9a44-3707c492b95c}" enabled="1" method="Privileged" siteId="{8619c67c-945a-48ae-8e77-35b1b71c9b98}" contentBits="0" removed="0"/>
+</clbl:labelList>
 </file>
</xml_diff>